<commit_message>
Generar Excel Memoria alumnos falta por rellenar de datos
</commit_message>
<xml_diff>
--- a/documentacion/plantillas/memoria alumno/MD750601 Memoria Final.xlsx
+++ b/documentacion/plantillas/memoria alumno/MD750601 Memoria Final.xlsx
@@ -158,13 +158,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -195,7 +199,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="topRight" activeCell="J2" activeCellId="0" sqref="J2"/>
       <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="C3" activeCellId="1" sqref="C2 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -203,7 +207,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="44.14"/>
@@ -213,7 +217,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -230,7 +234,7 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -250,7 +254,7 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>

</xml_diff>